<commit_message>
feat: enable cross schema inheritance
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/CohortsCentral.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/CohortsCentral.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C94721C-3C86-E248-8780-6B3A108280A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E621631F-C7C1-D046-936E-D2F48C21A32C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
+    <workbookView xWindow="400" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="StatusDetails" sheetId="17" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">molgenis!$A$1:$L$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">molgenis!$A$1:$L$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="384">
   <si>
     <t>name</t>
   </si>
@@ -1164,6 +1164,30 @@
   </si>
   <si>
     <t>missingValues</t>
+  </si>
+  <si>
+    <t>harmonisedTable,harmonisedVariable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in UI this is then one lookup field. In Excel it will be two columns. Value of 'targetVariable' is filtered based on selected 'targetCollection' and together be used for fkey(collection,table,name) in Variable. </t>
+  </si>
+  <si>
+    <t>match</t>
+  </si>
+  <si>
+    <t>e.g. 'complete, partial, planned, no-match'</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>whether harmonisation is still draft or final</t>
+  </si>
+  <si>
+    <t>AllVariableHarmonisations</t>
+  </si>
+  <si>
+    <t>harmonisedVariable</t>
   </si>
 </sst>
 </file>
@@ -1221,7 +1245,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1249,6 +1273,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1294,7 +1324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1315,6 +1345,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1634,11 +1665,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E080B8D-E59C-EC4A-8043-87277F816BB8}">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1692,72 +1723,87 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>383</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>329</v>
+      </c>
+      <c r="E2" s="20">
+        <v>1</v>
+      </c>
+      <c r="F2" s="20" t="s">
         <v>358</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="G2" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>378</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>329</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>362</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>380</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>329</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="J4" s="20" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>329</v>
-      </c>
-      <c r="E2" s="10">
-        <v>1</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>355</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>370</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>328</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="J4" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K4" s="20" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>358</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="6" t="b">
+      <c r="C5" s="10" t="s">
         <v>1</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1765,39 +1811,30 @@
         <v>358</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="J6" s="6" t="b">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6">
         <v>1</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>358</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>359</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>329</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>364</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>349</v>
+      <c r="C7" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>352</v>
       </c>
       <c r="J7" s="6" t="b">
         <v>1</v>
@@ -1808,19 +1845,13 @@
         <v>358</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>334</v>
+        <v>7</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>353</v>
+        <v>6</v>
       </c>
       <c r="J8" s="6" t="b">
         <v>1</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1828,36 +1859,42 @@
         <v>358</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>329</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="J9" s="6" t="b">
         <v>1</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>358</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>337</v>
+      <c r="C10" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>364</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>349</v>
       </c>
       <c r="J10" s="6" t="b">
         <v>1</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1865,16 +1902,19 @@
         <v>358</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>375</v>
+        <v>334</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>337</v>
+        <v>329</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>353</v>
       </c>
       <c r="J11" s="6" t="b">
         <v>1</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>372</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1882,25 +1922,19 @@
         <v>358</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>339</v>
+        <v>2</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>348</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>349</v>
+      <c r="F12" s="6" t="s">
+        <v>354</v>
       </c>
       <c r="J12" s="6" t="b">
         <v>1</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>340</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1908,16 +1942,16 @@
         <v>358</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>18</v>
+        <v>374</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>337</v>
       </c>
       <c r="J13" s="6" t="b">
         <v>1</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>331</v>
+        <v>371</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1925,166 +1959,175 @@
         <v>358</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>3</v>
+        <v>375</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>6</v>
+        <v>337</v>
       </c>
       <c r="J14" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+      <c r="K14" s="6" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
         <v>358</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="J15" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D18" s="12" t="s">
         <v>337</v>
       </c>
-      <c r="J15" s="12" t="b">
+      <c r="J18" s="12" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+    <row r="19" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
         <v>355</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C19" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D19" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E19" s="7">
         <v>1</v>
       </c>
-      <c r="K16" s="7" t="s">
+      <c r="K19" s="7" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+    <row r="20" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
         <v>355</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C20" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D20" s="10" t="s">
         <v>328</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F20" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="J17" s="10" t="b">
+      <c r="J20" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="K17" s="10" t="s">
+      <c r="K20" s="10" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+    <row r="21" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
         <v>355</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C21" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D21" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J18" s="10" t="b">
+      <c r="J21" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="K18" s="10" t="s">
+      <c r="K21" s="10" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
+    <row r="22" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
         <v>355</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C22" s="12" t="s">
         <v>341</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D22" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J19" s="12" t="b">
+      <c r="J22" s="12" t="b">
         <v>1</v>
       </c>
-      <c r="K19" s="12" t="s">
+      <c r="K22" s="12" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="15" t="s">
+    <row r="23" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="15" t="s">
         <v>350</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C23" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D23" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E23" s="15">
         <v>1</v>
       </c>
-      <c r="K20" s="15" t="s">
+      <c r="K23" s="15" t="s">
         <v>322</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
-        <v>350</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="J21" s="16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
-        <v>350</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>328</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>356</v>
-      </c>
-      <c r="J22" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="K22" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
-        <v>350</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>328</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>351</v>
-      </c>
-      <c r="J23" s="16" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
@@ -2092,176 +2135,178 @@
         <v>350</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="J24" s="16" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="14" t="s">
+    <row r="25" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
         <v>350</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>328</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>356</v>
+      </c>
+      <c r="J25" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K25" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>328</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>351</v>
+      </c>
+      <c r="J26" s="16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J27" s="16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="C28" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D28" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="J25" s="14" t="b">
+      <c r="J28" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="13" t="s">
+    <row r="29" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C29" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D29" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E29" s="13">
         <v>1</v>
       </c>
-      <c r="K26" s="13" t="s">
+      <c r="K29" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
+    <row r="30" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C30" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D30" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J27" s="13" t="b">
+      <c r="J30" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
+    <row r="31" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C31" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D31" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="J28" s="13" t="b">
+      <c r="J31" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="14" t="s">
+    <row r="32" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="14" t="s">
         <v>351</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C32" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D32" s="14" t="s">
         <v>328</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F32" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="J29" s="14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="17" t="s">
-        <v>357</v>
-      </c>
-      <c r="B30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="K30" s="17" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="18" t="s">
-        <v>357</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="18" t="s">
-        <v>357</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" s="18">
-        <v>2</v>
-      </c>
-      <c r="J32" s="18" t="b">
+      <c r="J32" s="14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>352</v>
-      </c>
-      <c r="B33" s="17" t="s">
         <v>357</v>
       </c>
+      <c r="B33" s="8"/>
       <c r="D33" s="8"/>
       <c r="K33" s="17" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="34" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>329</v>
-      </c>
-      <c r="F34" s="18" t="s">
-        <v>352</v>
-      </c>
-      <c r="J34" s="18" t="b">
+        <v>6</v>
+      </c>
+      <c r="E34" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>327</v>
-      </c>
-      <c r="F35" s="18" t="s">
-        <v>352</v>
-      </c>
-      <c r="I35" s="18" t="s">
-        <v>34</v>
+        <v>6</v>
+      </c>
+      <c r="E35" s="18">
+        <v>2</v>
       </c>
       <c r="J35" s="18" t="b">
         <v>1</v>
@@ -2269,69 +2314,118 @@
     </row>
     <row r="36" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="B36" s="17" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="17" t="s">
+      <c r="D36" s="8"/>
+      <c r="K36" s="17" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="J37" s="18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="I38" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="J38" s="18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="17" t="s">
         <v>362</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="17" t="s">
-        <v>356</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>357</v>
-      </c>
-      <c r="K38" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>357</v>
-      </c>
-      <c r="D39" s="9"/>
-    </row>
-    <row r="40" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="8" t="s">
-        <v>363</v>
       </c>
       <c r="B40" s="17" t="s">
         <v>357</v>
       </c>
-      <c r="D40" s="8"/>
     </row>
     <row r="41" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="8" t="s">
-        <v>354</v>
+      <c r="A41" s="17" t="s">
+        <v>356</v>
       </c>
       <c r="B41" s="17" t="s">
         <v>357</v>
       </c>
-      <c r="D41" s="8"/>
-    </row>
-    <row r="42" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="8" t="s">
+      <c r="K41" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>357</v>
+      </c>
+      <c r="D42" s="9"/>
+    </row>
+    <row r="43" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="8" t="s">
         <v>353</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B45" s="17" t="s">
         <v>357</v>
       </c>
-      <c r="D42" s="8"/>
+      <c r="D45" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L29" xr:uid="{05A83487-31A5-894A-B1C5-9D57C8ECFC86}"/>
+  <autoFilter ref="A1:L32" xr:uid="{05A83487-31A5-894A-B1C5-9D57C8ECFC86}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
feat: improving cohort schema
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/CohortsCentral.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/CohortsCentral.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E621631F-C7C1-D046-936E-D2F48C21A32C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191D84D5-E1BE-7545-B3CB-1405E1ADC339}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
+    <workbookView xWindow="400" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="5" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>
@@ -24,19 +24,28 @@
     <sheet name="StatusDetails" sheetId="17" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">molgenis!$A$1:$L$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">molgenis!$A$1:$L$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="377">
   <si>
     <t>name</t>
   </si>
@@ -116,9 +125,6 @@
     <t>targetPopulation</t>
   </si>
   <si>
-    <t>categorical</t>
-  </si>
-  <si>
     <t>LifeCycle</t>
   </si>
   <si>
@@ -998,12 +1004,6 @@
     <t>baseline</t>
   </si>
   <si>
-    <t>continous</t>
-  </si>
-  <si>
-    <t>integer</t>
-  </si>
-  <si>
     <t>e.g. 'baseline' of 'follow-up1' or … (unique within a collection)</t>
   </si>
   <si>
@@ -1166,28 +1166,16 @@
     <t>missingValues</t>
   </si>
   <si>
-    <t>harmonisedTable,harmonisedVariable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in UI this is then one lookup field. In Excel it will be two columns. Value of 'targetVariable' is filtered based on selected 'targetCollection' and together be used for fkey(collection,table,name) in Variable. </t>
-  </si>
-  <si>
-    <t>match</t>
-  </si>
-  <si>
-    <t>e.g. 'complete, partial, planned, no-match'</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>whether harmonisation is still draft or final</t>
-  </si>
-  <si>
-    <t>AllVariableHarmonisations</t>
-  </si>
-  <si>
-    <t>harmonisedVariable</t>
+    <t>Continuous</t>
+  </si>
+  <si>
+    <t>Categorical</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>String</t>
   </si>
 </sst>
 </file>
@@ -1245,7 +1233,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1273,12 +1261,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1324,7 +1306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1345,7 +1327,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1665,11 +1646,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E080B8D-E59C-EC4A-8043-87277F816BB8}">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1690,151 +1671,145 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
-        <v>382</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>383</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>329</v>
-      </c>
-      <c r="E2" s="20">
+    <row r="2" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="20" t="s">
-        <v>358</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>376</v>
-      </c>
-      <c r="H2" s="20" t="s">
+      <c r="D2" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="E2" s="10">
+        <v>1</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="K2" s="20" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
-        <v>382</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>378</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>329</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>362</v>
-      </c>
-      <c r="K3" s="20" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
-        <v>382</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>380</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>329</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>344</v>
-      </c>
-      <c r="J4" s="20" t="b">
+      <c r="J4" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="K4" s="20" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="C5" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="6" t="b">
         <v>1</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>329</v>
-      </c>
-      <c r="E5" s="10">
-        <v>1</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>355</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="6">
+        <v>326</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="J6" s="6" t="b">
         <v>1</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>370</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>328</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>352</v>
+        <v>355</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>346</v>
       </c>
       <c r="J7" s="6" t="b">
         <v>1</v>
@@ -1842,471 +1817,463 @@
     </row>
     <row r="8" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>7</v>
+        <v>331</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>6</v>
+        <v>326</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>350</v>
       </c>
       <c r="J8" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="K8" s="6" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="J9" s="6" t="b">
         <v>1</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>359</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>329</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>364</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>349</v>
+        <v>355</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>334</v>
       </c>
       <c r="J10" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="K10" s="6" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="11" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>334</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>353</v>
       </c>
       <c r="J11" s="6" t="b">
         <v>1</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>4</v>
+        <v>369</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>2</v>
+        <v>336</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>354</v>
+        <v>326</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>346</v>
       </c>
       <c r="J12" s="6" t="b">
         <v>1</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>5</v>
+        <v>337</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>337</v>
+        <v>329</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="J13" s="6" t="b">
         <v>1</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>375</v>
+        <v>3</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>337</v>
+        <v>6</v>
       </c>
       <c r="J14" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="K14" s="6" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="C15" s="6" t="s">
+    </row>
+    <row r="15" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="J15" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="7">
+        <v>1</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="J17" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="G15" s="6" t="s">
+    </row>
+    <row r="20" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="15">
+        <v>1</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>353</v>
+      </c>
+      <c r="J22" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="F23" s="16" t="s">
         <v>348</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>349</v>
-      </c>
-      <c r="J15" s="6" t="b">
+      <c r="J23" s="16" t="b">
         <v>1</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J17" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
-        <v>358</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>338</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="J18" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
-        <v>355</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="7">
-        <v>1</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
-        <v>355</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>328</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>352</v>
-      </c>
-      <c r="J20" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="K20" s="10" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
-        <v>355</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J21" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="K21" s="10" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
-        <v>355</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J22" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="K22" s="12" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="15" t="s">
-        <v>350</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="15">
-        <v>1</v>
-      </c>
-      <c r="K23" s="15" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="J24" s="16" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
-        <v>350</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>328</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>356</v>
-      </c>
-      <c r="J25" s="16" t="b">
+    <row r="25" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="K25" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="16" t="s">
-        <v>350</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>328</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>351</v>
-      </c>
-      <c r="J26" s="16" t="b">
+    </row>
+    <row r="26" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
-        <v>350</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J27" s="16" t="b">
+      <c r="K26" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J27" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="14" t="s">
-        <v>350</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="J28" s="14" t="b">
+    <row r="28" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="13" t="s">
-        <v>351</v>
-      </c>
-      <c r="C29" s="13" t="s">
+    <row r="29" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="14" t="s">
+        <v>348</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J29" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="K30" s="17" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C31" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D31" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E31" s="18">
         <v>1</v>
       </c>
-      <c r="K29" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="13" t="s">
-        <v>351</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" s="13" t="s">
+    </row>
+    <row r="32" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="J30" s="13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="13" t="s">
-        <v>351</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J31" s="13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="14" t="s">
-        <v>351</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>328</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="J32" s="14" t="b">
+      <c r="E32" s="18">
+        <v>2</v>
+      </c>
+      <c r="J32" s="18" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>357</v>
-      </c>
-      <c r="B33" s="8"/>
+        <v>349</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>354</v>
+      </c>
       <c r="D33" s="8"/>
       <c r="K33" s="17" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="34" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="18">
+        <v>326</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="J34" s="18" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" s="18">
-        <v>2</v>
+        <v>324</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="J35" s="18" t="b">
         <v>1</v>
@@ -2314,118 +2281,69 @@
     </row>
     <row r="36" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>357</v>
-      </c>
-      <c r="D36" s="8"/>
-      <c r="K36" s="17" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="18" t="s">
-        <v>352</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>329</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>352</v>
-      </c>
-      <c r="J37" s="18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="18" t="s">
-        <v>352</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D38" s="18" t="s">
-        <v>327</v>
-      </c>
-      <c r="F38" s="18" t="s">
-        <v>352</v>
-      </c>
-      <c r="I38" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="J38" s="18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="17" t="s">
-        <v>344</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>357</v>
-      </c>
+        <v>354</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="K38" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>354</v>
+      </c>
+      <c r="D39" s="9"/>
     </row>
     <row r="40" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="17" t="s">
-        <v>362</v>
+      <c r="A40" s="8" t="s">
+        <v>360</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>357</v>
-      </c>
+        <v>354</v>
+      </c>
+      <c r="D40" s="8"/>
     </row>
     <row r="41" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="17" t="s">
-        <v>356</v>
+      <c r="A41" s="8" t="s">
+        <v>351</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>357</v>
-      </c>
-      <c r="K41" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B42" s="19" t="s">
-        <v>357</v>
-      </c>
-      <c r="D42" s="9"/>
-    </row>
-    <row r="43" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>357</v>
-      </c>
-      <c r="D43" s="8"/>
-    </row>
-    <row r="44" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="B44" s="17" t="s">
-        <v>357</v>
-      </c>
-      <c r="D44" s="8"/>
-    </row>
-    <row r="45" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>357</v>
-      </c>
-      <c r="D45" s="8"/>
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="D42" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L32" xr:uid="{05A83487-31A5-894A-B1C5-9D57C8ECFC86}"/>
+  <autoFilter ref="A1:L29" xr:uid="{05A83487-31A5-894A-B1C5-9D57C8ECFC86}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2462,10 +2380,10 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
@@ -2474,107 +2392,107 @@
         <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>315</v>
+      </c>
+      <c r="B3" t="s">
         <v>316</v>
       </c>
-      <c r="B3" t="s">
-        <v>317</v>
-      </c>
       <c r="C3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D3" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D4" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>318</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" t="s">
-        <v>319</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
       <c r="G5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H5" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>318</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
         <v>32</v>
       </c>
-      <c r="C6" t="s">
-        <v>319</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
       <c r="G6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H6" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -2607,10 +2525,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -2642,34 +2560,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -2694,22 +2612,22 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -2721,8 +2639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703D612C-4371-694D-BFA7-05A6222D28C0}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2734,27 +2652,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>374</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>320</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>321</v>
+        <v>375</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -2781,2139 +2699,2139 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B58" s="4"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59" s="4"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B186" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B187" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B188" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B191" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B194" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B195" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B196" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B197" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B210" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B211" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B213" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B214" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B215" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B221" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B222" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B223" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B231" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B232" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B234" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B235" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B236" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B237" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B238" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B239" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B240" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B241" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B242" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B243" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B244" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B245" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B247" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B248" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B249" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B250" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B251" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B252" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B253" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B254" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B255" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B256" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B257" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B258" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B259" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B260" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B261" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B262" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B263" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B264" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B265" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B266" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B267" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B268" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B269" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -4938,12 +4856,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
@@ -4971,17 +4889,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: replaced default search from 'text' to 'trigram' to allow for typos to still yield results
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-io/src/test/resources/CohortsCentral.xlsx
+++ b/backend/molgenis-emx2-io/src/test/resources/CohortsCentral.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/git/molgenis-emx2/backend/molgenis-emx2-io/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B962BB-6630-4E4A-AF7E-63929627F71B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680E6F36-E1B4-5B4E-8D83-00BC7E7A0CC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="33580" windowHeight="20540" firstSheet="2" activeTab="3" xr2:uid="{F42F3E6F-6A7C-5B4F-AA42-4152A61B026F}"/>
   </bookViews>
   <sheets>
     <sheet name="molgenis" sheetId="1" r:id="rId1"/>
-    <sheet name="Organisations" sheetId="20" r:id="rId2"/>
+    <sheet name="Providers" sheetId="20" r:id="rId2"/>
     <sheet name="Networks" sheetId="22" r:id="rId3"/>
     <sheet name="Collections" sheetId="2" r:id="rId4"/>
     <sheet name="Datasets" sheetId="3" r:id="rId5"/>
@@ -36,7 +36,7 @@
     <sheet name="StatusDetails" sheetId="11" r:id="rId21"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">molgenis!$A$1:$L$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">molgenis!$A$1:$L$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3675" uniqueCount="1153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3671" uniqueCount="1152">
   <si>
     <t>name</t>
   </si>
@@ -3244,9 +3244,6 @@
     <t>targetCollection,targetDataset,sourceCollection,sourceDataset</t>
   </si>
   <si>
-    <t>Organisations</t>
-  </si>
-  <si>
     <t>calculated field</t>
   </si>
   <si>
@@ -3484,9 +3481,6 @@
     <t>outcomes</t>
   </si>
   <si>
-    <t>partners</t>
-  </si>
-  <si>
     <t>use when same variable is repeated</t>
   </si>
   <si>
@@ -3578,6 +3572,9 @@
   </si>
   <si>
     <t>ISGlobal</t>
+  </si>
+  <si>
+    <t>Providers</t>
   </si>
 </sst>
 </file>
@@ -4216,11 +4213,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E080B8D-E59C-EC4A-8043-87277F816BB8}">
-  <dimension ref="A1:K122"/>
+  <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" activeCellId="1" sqref="C63 C25"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4276,7 +4273,7 @@
     </row>
     <row r="2" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>63</v>
@@ -4290,7 +4287,7 @@
     </row>
     <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>0</v>
@@ -4310,7 +4307,7 @@
     </row>
     <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>789</v>
@@ -4324,7 +4321,7 @@
     </row>
     <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>64</v>
@@ -4344,36 +4341,33 @@
     </row>
     <row r="6" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>1041</v>
+        <v>1151</v>
       </c>
       <c r="J6" s="5" t="b">
         <v>1</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>1121</v>
+        <v>2</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>1041</v>
+        <v>8</v>
       </c>
       <c r="J7" s="5" t="b">
         <v>1</v>
@@ -4381,13 +4375,13 @@
     </row>
     <row r="8" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J8" s="5" t="b">
         <v>1</v>
@@ -4395,13 +4389,16 @@
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>66</v>
+        <v>790</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>5</v>
+        <v>24</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="J9" s="5" t="b">
         <v>1</v>
@@ -4409,10 +4406,10 @@
     </row>
     <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>790</v>
+        <v>67</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>24</v>
@@ -4426,16 +4423,13 @@
     </row>
     <row r="11" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>67</v>
+        <v>879</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>78</v>
+        <v>881</v>
       </c>
       <c r="J11" s="5" t="b">
         <v>1</v>
@@ -4443,10 +4437,10 @@
     </row>
     <row r="12" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>881</v>
@@ -4457,13 +4451,13 @@
     </row>
     <row r="13" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>880</v>
+        <v>793</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>881</v>
+        <v>8</v>
       </c>
       <c r="J13" s="5" t="b">
         <v>1</v>
@@ -4471,13 +4465,13 @@
     </row>
     <row r="14" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>793</v>
+        <v>1111</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J14" s="5" t="b">
         <v>1</v>
@@ -4485,24 +4479,27 @@
     </row>
     <row r="15" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>1112</v>
+        <v>813</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J15" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="K15" s="5" t="s">
+        <v>1024</v>
+      </c>
     </row>
     <row r="16" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>8</v>
@@ -4510,16 +4507,13 @@
       <c r="J16" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="K16" s="5" t="s">
-        <v>1024</v>
-      </c>
     </row>
     <row r="17" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>8</v>
@@ -4530,121 +4524,124 @@
     </row>
     <row r="18" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>815</v>
+        <v>898</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>8</v>
+        <v>23</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>885</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>909</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="J18" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="K18" s="5" t="s">
+        <v>1041</v>
+      </c>
     </row>
     <row r="19" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>1140</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>898</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>885</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>909</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="J19" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K19" s="5" t="s">
-        <v>1042</v>
+        <v>77</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>1138</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>1140</v>
+      <c r="C20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>1114</v>
+      </c>
+      <c r="J20" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>1117</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>1115</v>
-      </c>
-      <c r="J21" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>1118</v>
+        <v>1114</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>1138</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>1115</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>1140</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>1115</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>1051</v>
-      </c>
-      <c r="D23" s="5" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G22" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="J23" s="5" t="b">
+      <c r="J22" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="55" t="s">
+    <row r="23" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="55" t="s">
         <v>885</v>
       </c>
-      <c r="C24" s="55" t="s">
+      <c r="C23" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="55" t="s">
+      <c r="D23" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="55">
+      <c r="E23" s="55">
         <v>1</v>
       </c>
-      <c r="F24" s="55" t="s">
-        <v>1140</v>
-      </c>
-      <c r="K24" s="55" t="s">
+      <c r="F23" s="55" t="s">
+        <v>1138</v>
+      </c>
+      <c r="K23" s="55" t="s">
         <v>843</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="52" t="s">
+        <v>885</v>
+      </c>
+      <c r="C24" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="52">
+        <v>1</v>
+      </c>
+      <c r="K24" s="52" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.2">
@@ -4652,30 +4649,33 @@
         <v>885</v>
       </c>
       <c r="C25" s="52" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D25" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="52">
+      <c r="J25" s="52" t="b">
         <v>1</v>
       </c>
-      <c r="K25" s="52" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="52" t="s">
         <v>885</v>
       </c>
-      <c r="C26" s="52" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="J26" s="52" t="b">
+      <c r="C26" s="50" t="s">
+        <v>488</v>
+      </c>
+      <c r="D26" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="J26" s="50" t="b">
         <v>1</v>
+      </c>
+      <c r="K26" s="50" t="s">
+        <v>899</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.2">
@@ -4683,19 +4683,16 @@
         <v>885</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>488</v>
+        <v>2</v>
       </c>
       <c r="D27" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" s="50" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="J27" s="50" t="b">
         <v>1</v>
       </c>
       <c r="K27" s="50" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.2">
@@ -4703,16 +4700,25 @@
         <v>885</v>
       </c>
       <c r="C28" s="50" t="s">
-        <v>2</v>
+        <v>1025</v>
       </c>
       <c r="D28" s="50" t="s">
-        <v>8</v>
+        <v>24</v>
+      </c>
+      <c r="F28" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="H28" s="50" t="s">
+        <v>907</v>
+      </c>
+      <c r="I28" s="50" t="s">
+        <v>72</v>
       </c>
       <c r="J28" s="50" t="b">
         <v>1</v>
       </c>
       <c r="K28" s="50" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.2">
@@ -4720,25 +4726,16 @@
         <v>885</v>
       </c>
       <c r="C29" s="50" t="s">
-        <v>1025</v>
+        <v>840</v>
       </c>
       <c r="D29" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="F29" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="H29" s="50" t="s">
-        <v>907</v>
-      </c>
-      <c r="I29" s="50" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="J29" s="50" t="b">
         <v>1</v>
       </c>
       <c r="K29" s="50" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.2">
@@ -4746,7 +4743,7 @@
         <v>885</v>
       </c>
       <c r="C30" s="50" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="D30" s="50" t="s">
         <v>8</v>
@@ -4755,7 +4752,7 @@
         <v>1</v>
       </c>
       <c r="K30" s="50" t="s">
-        <v>901</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.2">
@@ -4763,7 +4760,7 @@
         <v>885</v>
       </c>
       <c r="C31" s="50" t="s">
-        <v>841</v>
+        <v>815</v>
       </c>
       <c r="D31" s="50" t="s">
         <v>8</v>
@@ -4772,7 +4769,7 @@
         <v>1</v>
       </c>
       <c r="K31" s="50" t="s">
-        <v>1033</v>
+        <v>812</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.2">
@@ -4780,71 +4777,71 @@
         <v>885</v>
       </c>
       <c r="C32" s="50" t="s">
-        <v>815</v>
+        <v>489</v>
       </c>
       <c r="D32" s="50" t="s">
-        <v>8</v>
+        <v>23</v>
+      </c>
+      <c r="F32" s="50" t="s">
+        <v>896</v>
+      </c>
+      <c r="G32" s="50" t="s">
+        <v>895</v>
+      </c>
+      <c r="H32" s="50" t="s">
+        <v>1039</v>
+      </c>
+      <c r="I32" s="50" t="s">
+        <v>1040</v>
       </c>
       <c r="J32" s="50" t="b">
         <v>1</v>
       </c>
-      <c r="K32" s="50" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="52" t="s">
+    </row>
+    <row r="33" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="51" t="s">
         <v>885</v>
       </c>
-      <c r="C33" s="50" t="s">
-        <v>489</v>
-      </c>
-      <c r="D33" s="50" t="s">
+      <c r="C33" s="51" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="F33" s="50" t="s">
-        <v>896</v>
-      </c>
-      <c r="G33" s="50" t="s">
-        <v>895</v>
-      </c>
-      <c r="H33" s="50" t="s">
-        <v>1039</v>
-      </c>
-      <c r="I33" s="50" t="s">
-        <v>1040</v>
-      </c>
-      <c r="J33" s="50" t="b">
+      <c r="F33" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="51" t="s">
+        <v>887</v>
+      </c>
+      <c r="H33" s="51" t="s">
+        <v>897</v>
+      </c>
+      <c r="I33" s="51" t="s">
+        <v>891</v>
+      </c>
+      <c r="J33" s="51" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="51" t="s">
-        <v>885</v>
-      </c>
-      <c r="C34" s="51" t="s">
-        <v>155</v>
-      </c>
-      <c r="D34" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="F34" s="51" t="s">
+      <c r="K33" s="51" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G34" s="51" t="s">
-        <v>887</v>
-      </c>
-      <c r="H34" s="51" t="s">
-        <v>897</v>
-      </c>
-      <c r="I34" s="51" t="s">
-        <v>891</v>
-      </c>
-      <c r="J34" s="51" t="b">
+      <c r="C34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="5">
         <v>1</v>
       </c>
-      <c r="K34" s="51" t="s">
-        <v>842</v>
+      <c r="F34" s="5" t="s">
+        <v>1138</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -4852,7 +4849,7 @@
         <v>50</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>7</v>
+        <v>887</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>25</v>
@@ -4861,7 +4858,13 @@
         <v>1</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>1140</v>
+        <v>885</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>886</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -4869,22 +4872,16 @@
         <v>50</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>887</v>
+        <v>0</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E36" s="5">
         <v>1</v>
       </c>
-      <c r="F36" s="5" t="s">
-        <v>885</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>886</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>72</v>
+      <c r="K36" s="5" t="s">
+        <v>888</v>
       </c>
     </row>
     <row r="37" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -4892,16 +4889,25 @@
         <v>50</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="5">
+        <v>25</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>903</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>891</v>
+      </c>
+      <c r="J37" s="5" t="b">
         <v>1</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>888</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -4909,25 +4915,25 @@
         <v>50</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>903</v>
+        <v>73</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>891</v>
+        <v>72</v>
       </c>
       <c r="J38" s="5" t="b">
         <v>1</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>1122</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -4935,25 +4941,13 @@
         <v>50</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="J39" s="5" t="b">
         <v>1</v>
-      </c>
-      <c r="K39" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -4961,13 +4955,19 @@
         <v>50</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>5</v>
+        <v>25</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="J40" s="5" t="b">
         <v>1</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -4975,19 +4975,19 @@
         <v>50</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J41" s="5" t="b">
         <v>1</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -4995,19 +4995,16 @@
         <v>50</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>25</v>
+        <v>488</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J42" s="5" t="b">
         <v>1</v>
-      </c>
-      <c r="K42" s="5" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -5015,16 +5012,25 @@
         <v>50</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>488</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>24</v>
+        <v>76</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>40</v>
+        <v>50</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>904</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>891</v>
       </c>
       <c r="J43" s="5" t="b">
         <v>1</v>
+      </c>
+      <c r="K43" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -5032,25 +5038,16 @@
         <v>50</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>904</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>891</v>
+        <v>28</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="J44" s="5" t="b">
         <v>1</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -5058,16 +5055,13 @@
         <v>50</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="J45" s="5" t="b">
         <v>1</v>
-      </c>
-      <c r="K45" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -5075,30 +5069,30 @@
         <v>50</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J46" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K46" s="5" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J47" s="5" t="b">
+      <c r="C47" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J47" s="14" t="b">
         <v>1</v>
-      </c>
-      <c r="K47" s="5" t="s">
-        <v>817</v>
       </c>
     </row>
     <row r="48" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -5106,221 +5100,221 @@
         <v>50</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>32</v>
+        <v>489</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G48" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H48" s="14" t="s">
+        <v>905</v>
+      </c>
+      <c r="I48" s="14" t="s">
+        <v>908</v>
       </c>
       <c r="J48" s="14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K48" s="14" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C49" s="14" t="s">
-        <v>489</v>
-      </c>
-      <c r="D49" s="14" t="s">
+      <c r="C49" s="5" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F49" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="G49" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="H49" s="14" t="s">
-        <v>905</v>
-      </c>
-      <c r="I49" s="14" t="s">
-        <v>908</v>
-      </c>
-      <c r="J49" s="14" t="b">
+      <c r="F49" s="5" t="s">
+        <v>1107</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>1108</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>1115</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>1116</v>
+      </c>
+      <c r="J49" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="K49" s="14" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="5" t="s">
+    </row>
+    <row r="50" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="55" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C50" s="55" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D50" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="E50" s="55">
+        <v>1</v>
+      </c>
+      <c r="F50" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>1111</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>1108</v>
-      </c>
-      <c r="G50" s="5" t="s">
+      <c r="H50" s="55" t="s">
         <v>1109</v>
       </c>
-      <c r="H50" s="5" t="s">
-        <v>1116</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>1117</v>
-      </c>
-      <c r="J50" s="5" t="b">
+      <c r="I50" s="55" t="s">
+        <v>891</v>
+      </c>
+      <c r="K50" s="55" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="52" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C51" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="D51" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="52">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="55" t="s">
-        <v>1108</v>
-      </c>
-      <c r="C51" s="55" t="s">
-        <v>1109</v>
-      </c>
-      <c r="D51" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="E51" s="55">
-        <v>1</v>
-      </c>
-      <c r="F51" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="H51" s="55" t="s">
-        <v>1110</v>
-      </c>
-      <c r="I51" s="55" t="s">
-        <v>891</v>
-      </c>
-      <c r="K51" s="55" t="s">
-        <v>48</v>
+      <c r="K51" s="52" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="52" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="C52" s="52" t="s">
-        <v>127</v>
+        <v>6</v>
       </c>
       <c r="D52" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E52" s="52">
-        <v>1</v>
-      </c>
-      <c r="K52" s="52" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="53" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="52" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="C53" s="52" t="s">
-        <v>6</v>
+        <v>128</v>
       </c>
       <c r="D53" s="52" t="s">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="J53" s="52" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="52" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="C54" s="52" t="s">
-        <v>128</v>
+        <v>1106</v>
       </c>
       <c r="D54" s="52" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J54" s="52" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="52" t="s">
-        <v>1108</v>
-      </c>
-      <c r="C55" s="52" t="s">
+    <row r="55" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="51" t="s">
         <v>1107</v>
       </c>
-      <c r="D55" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="J55" s="52" t="b">
+      <c r="C55" s="51" t="s">
+        <v>136</v>
+      </c>
+      <c r="D55" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="J55" s="51" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="51" t="s">
-        <v>1108</v>
-      </c>
-      <c r="C56" s="51" t="s">
-        <v>136</v>
-      </c>
-      <c r="D56" s="51" t="s">
+    <row r="56" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="53" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D56" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="J56" s="51" t="b">
+      <c r="E56" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="53" t="s">
-        <v>1041</v>
+        <v>1151</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="D57" s="12" t="s">
         <v>5</v>
       </c>
       <c r="E57" s="12">
+        <v>2</v>
+      </c>
+      <c r="J57" s="12" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="53" t="s">
-        <v>1041</v>
+        <v>1151</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>0</v>
+        <v>789</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E58" s="12">
-        <v>2</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="E58" s="12"/>
       <c r="J58" s="12" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="53" t="s">
-        <v>1041</v>
+        <v>1151</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>789</v>
+        <v>2</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E59" s="12"/>
+        <v>8</v>
+      </c>
       <c r="J59" s="12" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="53" t="s">
-        <v>1041</v>
+        <v>1151</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J60" s="12" t="b">
         <v>1</v>
@@ -5328,13 +5322,16 @@
     </row>
     <row r="61" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="53" t="s">
-        <v>1041</v>
+        <v>1151</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>66</v>
+        <v>790</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>5</v>
+        <v>24</v>
+      </c>
+      <c r="F61" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="J61" s="12" t="b">
         <v>1</v>
@@ -5342,57 +5339,55 @@
     </row>
     <row r="62" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="53" t="s">
-        <v>1041</v>
+        <v>1151</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>790</v>
+        <v>1139</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>78</v>
+        <v>1138</v>
+      </c>
+      <c r="G62" s="12" t="s">
+        <v>1136</v>
       </c>
       <c r="J62" s="12" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="53" t="s">
-        <v>1041</v>
-      </c>
-      <c r="C63" s="12" t="s">
-        <v>1141</v>
-      </c>
-      <c r="D63" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F63" s="12" t="s">
-        <v>1140</v>
-      </c>
-      <c r="G63" s="12" t="s">
-        <v>1138</v>
-      </c>
-      <c r="J63" s="12" t="b">
+    <row r="63" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="13" t="s">
+      <c r="J63" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="B64" s="13"/>
-      <c r="C64" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D64" s="13" t="s">
+      <c r="B64" s="18"/>
+      <c r="C64" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E64" s="4">
-        <v>1</v>
-      </c>
-      <c r="J64" s="4" t="b">
-        <v>1</v>
+      <c r="E64" s="19">
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -5401,13 +5396,16 @@
       </c>
       <c r="B65" s="18"/>
       <c r="C65" s="18" t="s">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="D65" s="18" t="s">
         <v>5</v>
       </c>
       <c r="E65" s="19">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="J65" s="19" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -5416,13 +5414,10 @@
       </c>
       <c r="B66" s="18"/>
       <c r="C66" s="18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E66" s="19">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J66" s="19" t="b">
         <v>1</v>
@@ -5433,8 +5428,8 @@
         <v>78</v>
       </c>
       <c r="B67" s="18"/>
-      <c r="C67" s="18" t="s">
-        <v>80</v>
+      <c r="C67" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="D67" s="18" t="s">
         <v>8</v>
@@ -5443,98 +5438,103 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B68" s="18"/>
-      <c r="C68" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D68" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="J68" s="19" t="b">
+    <row r="68" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E68" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
-        <v>1142</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E69" s="4">
+    <row r="69" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="19" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D69" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E69" s="19">
         <v>1</v>
+      </c>
+      <c r="F69" s="19" t="s">
+        <v>1138</v>
       </c>
     </row>
     <row r="70" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="19" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="C70" s="19" t="s">
-        <v>1143</v>
+        <v>69</v>
       </c>
       <c r="D70" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="E70" s="19">
+        <v>5</v>
+      </c>
+      <c r="J70" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="F70" s="19" t="s">
-        <v>1140</v>
+      <c r="K70" s="19" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="19" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D71" s="19" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="J71" s="19" t="b">
         <v>1</v>
       </c>
       <c r="K71" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="19" t="s">
-        <v>1142</v>
-      </c>
-      <c r="C72" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="D72" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="J72" s="19" t="b">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="60" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C72" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="J72" s="60" t="b">
         <v>1</v>
       </c>
-      <c r="K72" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="60" t="s">
-        <v>1142</v>
-      </c>
-      <c r="C73" s="60" t="s">
-        <v>2</v>
-      </c>
-      <c r="D73" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="J73" s="60" t="b">
+    </row>
+    <row r="73" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C73" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E73" s="15">
         <v>1</v>
+      </c>
+      <c r="F73" s="15" t="s">
+        <v>1138</v>
+      </c>
+      <c r="K73" s="15" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="74" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -5542,36 +5542,30 @@
         <v>38</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E74" s="15">
         <v>1</v>
       </c>
-      <c r="F74" s="15" t="s">
-        <v>1140</v>
-      </c>
       <c r="K74" s="15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="15" t="s">
+    <row r="75" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C75" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D75" s="15" t="s">
+      <c r="C75" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D75" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E75" s="15">
+      <c r="J75" s="10" t="b">
         <v>1</v>
-      </c>
-      <c r="K75" s="15" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="76" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -5579,40 +5573,43 @@
         <v>38</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>2</v>
+        <v>791</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J76" s="10" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="10" t="s">
+    <row r="77" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C77" s="10" t="s">
-        <v>791</v>
-      </c>
-      <c r="D77" s="10" t="s">
+      <c r="C77" s="15" t="s">
+        <v>792</v>
+      </c>
+      <c r="D77" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J77" s="10" t="b">
+      <c r="J77" s="15" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="15" t="s">
+    <row r="78" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C78" s="15" t="s">
-        <v>792</v>
-      </c>
-      <c r="D78" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J78" s="15" t="b">
+      <c r="C78" s="10" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D78" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F78" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J78" s="10" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5621,7 +5618,7 @@
         <v>38</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="D79" s="10" t="s">
         <v>25</v>
@@ -5638,16 +5635,25 @@
         <v>38</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F80" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="H80" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I80" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="J80" s="10" t="b">
         <v>1</v>
+      </c>
+      <c r="K80" s="10" t="s">
+        <v>1029</v>
       </c>
     </row>
     <row r="81" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -5655,25 +5661,13 @@
         <v>38</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>1025</v>
+        <v>1010</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F81" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="H81" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="I81" s="10" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="J81" s="10" t="b">
         <v>1</v>
-      </c>
-      <c r="K81" s="10" t="s">
-        <v>1029</v>
       </c>
     </row>
     <row r="82" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -5681,13 +5675,16 @@
         <v>38</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>1010</v>
+        <v>1023</v>
       </c>
       <c r="D82" s="10" t="s">
         <v>8</v>
       </c>
       <c r="J82" s="10" t="b">
         <v>1</v>
+      </c>
+      <c r="K82" s="10" t="s">
+        <v>1028</v>
       </c>
     </row>
     <row r="83" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -5695,7 +5692,7 @@
         <v>38</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>1023</v>
+        <v>1030</v>
       </c>
       <c r="D83" s="10" t="s">
         <v>8</v>
@@ -5704,38 +5701,41 @@
         <v>1</v>
       </c>
       <c r="K83" s="10" t="s">
-        <v>1028</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="10" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C84" s="10" t="s">
-        <v>1030</v>
-      </c>
-      <c r="D84" s="10" t="s">
+      <c r="C84" s="11" t="s">
+        <v>815</v>
+      </c>
+      <c r="D84" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J84" s="10" t="b">
+      <c r="J84" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="K84" s="10" t="s">
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C85" s="11" t="s">
-        <v>815</v>
-      </c>
-      <c r="D85" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="J85" s="11" t="b">
+    </row>
+    <row r="85" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E85" s="10">
         <v>1</v>
+      </c>
+      <c r="F85" s="10" t="s">
+        <v>1138</v>
+      </c>
+      <c r="K85" s="10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="86" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -5743,16 +5743,13 @@
         <v>39</v>
       </c>
       <c r="C86" s="10" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E86" s="10">
         <v>1</v>
-      </c>
-      <c r="F86" s="10" t="s">
-        <v>1140</v>
       </c>
       <c r="K86" s="10" t="s">
         <v>13</v>
@@ -5763,16 +5760,13 @@
         <v>39</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E87" s="10">
+        <v>10</v>
+      </c>
+      <c r="J87" s="10" t="b">
         <v>1</v>
-      </c>
-      <c r="K87" s="10" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -5780,26 +5774,29 @@
         <v>39</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J88" s="10" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="10" t="s">
+    <row r="89" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C89" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D89" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="J89" s="10" t="b">
+      <c r="C89" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D89" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F89" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J89" s="15" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5808,16 +5805,13 @@
         <v>39</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>14</v>
+        <v>877</v>
       </c>
       <c r="D90" s="15" t="s">
         <v>24</v>
       </c>
       <c r="F90" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="J90" s="15" t="b">
-        <v>1</v>
+        <v>882</v>
       </c>
     </row>
     <row r="91" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -5825,7 +5819,7 @@
         <v>39</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>877</v>
+        <v>1113</v>
       </c>
       <c r="D91" s="15" t="s">
         <v>24</v>
@@ -5833,39 +5827,51 @@
       <c r="F91" s="15" t="s">
         <v>882</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="15" t="s">
+      <c r="J91" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K91" s="15" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C92" s="15" t="s">
-        <v>1114</v>
-      </c>
-      <c r="D92" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F92" s="15" t="s">
-        <v>882</v>
-      </c>
-      <c r="J92" s="15" t="b">
+      <c r="C92" s="11" t="s">
+        <v>815</v>
+      </c>
+      <c r="D92" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J92" s="11" t="b">
         <v>1</v>
       </c>
-      <c r="K92" s="15" t="s">
-        <v>1113</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C93" s="11" t="s">
-        <v>815</v>
-      </c>
-      <c r="D93" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="J93" s="11" t="b">
+    </row>
+    <row r="93" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E93" s="6">
         <v>1</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H93" s="6" t="s">
+        <v>890</v>
+      </c>
+      <c r="I93" s="6" t="s">
+        <v>891</v>
+      </c>
+      <c r="K93" s="6" t="s">
+        <v>906</v>
       </c>
     </row>
     <row r="94" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -5873,7 +5879,7 @@
         <v>52</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>53</v>
+        <v>889</v>
       </c>
       <c r="D94" s="6" t="s">
         <v>25</v>
@@ -5882,16 +5888,13 @@
         <v>1</v>
       </c>
       <c r="F94" s="6" t="s">
-        <v>50</v>
+        <v>885</v>
       </c>
       <c r="H94" s="6" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="I94" s="6" t="s">
-        <v>891</v>
-      </c>
-      <c r="K94" s="6" t="s">
-        <v>906</v>
+        <v>72</v>
       </c>
     </row>
     <row r="95" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -5899,22 +5902,16 @@
         <v>52</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>889</v>
+        <v>54</v>
       </c>
       <c r="D95" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E95" s="6">
-        <v>1</v>
-      </c>
       <c r="F95" s="6" t="s">
-        <v>885</v>
-      </c>
-      <c r="H95" s="6" t="s">
-        <v>892</v>
-      </c>
-      <c r="I95" s="6" t="s">
-        <v>72</v>
+        <v>44</v>
+      </c>
+      <c r="K95" s="6" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="96" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -5922,16 +5919,19 @@
         <v>52</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D96" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F96" s="6" t="s">
-        <v>44</v>
+        <v>34</v>
+      </c>
+      <c r="J96" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="K96" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="97" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -5939,19 +5939,25 @@
         <v>52</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F97" s="6" t="s">
-        <v>34</v>
+        <v>50</v>
+      </c>
+      <c r="H97" s="6" t="s">
+        <v>893</v>
+      </c>
+      <c r="I97" s="6" t="s">
+        <v>891</v>
       </c>
       <c r="J97" s="6" t="b">
         <v>1</v>
       </c>
       <c r="K97" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="98" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -5959,25 +5965,16 @@
         <v>52</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F98" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H98" s="6" t="s">
-        <v>893</v>
-      </c>
-      <c r="I98" s="6" t="s">
-        <v>891</v>
+        <v>8</v>
       </c>
       <c r="J98" s="6" t="b">
         <v>1</v>
       </c>
       <c r="K98" s="6" t="s">
-        <v>59</v>
+        <v>818</v>
       </c>
     </row>
     <row r="99" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -5985,7 +5982,7 @@
         <v>52</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>2</v>
+        <v>811</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>8</v>
@@ -5994,7 +5991,7 @@
         <v>1</v>
       </c>
       <c r="K99" s="6" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
     </row>
     <row r="100" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -6002,7 +5999,7 @@
         <v>52</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>811</v>
+        <v>60</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>8</v>
@@ -6011,46 +6008,52 @@
         <v>1</v>
       </c>
       <c r="K100" s="6" t="s">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D101" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J101" s="6" t="b">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="7" t="s">
+        <v>896</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>895</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E101" s="7">
         <v>1</v>
       </c>
-      <c r="K101" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="7" t="s">
+      <c r="F101" s="7" t="s">
+        <v>885</v>
+      </c>
+      <c r="H101" s="7" t="s">
+        <v>894</v>
+      </c>
+      <c r="I101" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="16" t="s">
         <v>896</v>
       </c>
-      <c r="C102" s="7" t="s">
-        <v>895</v>
-      </c>
-      <c r="D102" s="7" t="s">
+      <c r="C102" s="16" t="s">
+        <v>889</v>
+      </c>
+      <c r="D102" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E102" s="7">
+      <c r="E102" s="16">
         <v>1</v>
       </c>
-      <c r="F102" s="7" t="s">
+      <c r="F102" s="16" t="s">
         <v>885</v>
       </c>
-      <c r="H102" s="7" t="s">
-        <v>894</v>
-      </c>
-      <c r="I102" s="8" t="s">
+      <c r="H102" s="16" t="s">
+        <v>892</v>
+      </c>
+      <c r="I102" s="17" t="s">
         <v>72</v>
       </c>
     </row>
@@ -6059,22 +6062,20 @@
         <v>896</v>
       </c>
       <c r="C103" s="16" t="s">
-        <v>889</v>
+        <v>128</v>
       </c>
       <c r="D103" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E103" s="16">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F103" s="16" t="s">
         <v>885</v>
       </c>
-      <c r="H103" s="16" t="s">
-        <v>892</v>
-      </c>
-      <c r="I103" s="17" t="s">
-        <v>72</v>
+      <c r="I103" s="17"/>
+      <c r="J103" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K103" s="16" t="s">
+        <v>1036</v>
       </c>
     </row>
     <row r="104" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
@@ -6082,58 +6083,51 @@
         <v>896</v>
       </c>
       <c r="C104" s="16" t="s">
-        <v>128</v>
+        <v>2</v>
       </c>
       <c r="D104" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F104" s="16" t="s">
-        <v>885</v>
-      </c>
-      <c r="I104" s="17"/>
+        <v>8</v>
+      </c>
       <c r="J104" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="K104" s="16" t="s">
-        <v>1036</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="16" t="s">
+    </row>
+    <row r="105" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="9" t="s">
         <v>896</v>
       </c>
-      <c r="C105" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D105" s="16" t="s">
+      <c r="C105" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D105" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J105" s="16" t="b">
+      <c r="J105" s="9" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="9" t="s">
-        <v>896</v>
-      </c>
-      <c r="C106" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D106" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J106" s="9" t="b">
-        <v>1</v>
+    <row r="106" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="B106" s="21"/>
+      <c r="D106" s="21"/>
+      <c r="K106" s="12" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="107" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="B107" s="21"/>
-      <c r="D107" s="21"/>
-      <c r="K107" s="12" t="s">
-        <v>204</v>
+      <c r="C107" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D107" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E107" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -6141,12 +6135,12 @@
         <v>203</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="D108" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E108" s="12">
+        <v>10</v>
+      </c>
+      <c r="J108" s="12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6155,42 +6149,45 @@
         <v>203</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>128</v>
+        <v>205</v>
       </c>
       <c r="D109" s="12" t="s">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="E109" s="12">
+        <v>2</v>
       </c>
       <c r="J109" s="12" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="12" t="s">
+    <row r="110" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B110" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C110" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="D110" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E110" s="12">
-        <v>2</v>
-      </c>
-      <c r="J110" s="12" t="b">
+      <c r="D110" s="13"/>
+      <c r="K110" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C111" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D111" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F111" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J111" s="12" t="b">
         <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B111" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="D111" s="13"/>
-      <c r="K111" s="4" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="112" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -6198,13 +6195,22 @@
         <v>40</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D112" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F112" s="12" t="s">
-        <v>40</v>
+        <v>50</v>
+      </c>
+      <c r="G112" s="12" t="s">
+        <v>488</v>
+      </c>
+      <c r="H112" s="12" t="s">
+        <v>897</v>
+      </c>
+      <c r="I112" s="12" t="s">
+        <v>891</v>
       </c>
       <c r="J112" s="12" t="b">
         <v>1</v>
@@ -6215,50 +6221,32 @@
         <v>40</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D113" s="12" t="s">
         <v>23</v>
       </c>
       <c r="F113" s="12" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G113" s="12" t="s">
-        <v>488</v>
-      </c>
-      <c r="H113" s="12" t="s">
-        <v>897</v>
-      </c>
-      <c r="I113" s="12" t="s">
-        <v>891</v>
+        <v>153</v>
       </c>
       <c r="J113" s="12" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C114" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="D114" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F114" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G114" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="J114" s="12" t="b">
-        <v>1</v>
+    <row r="114" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="115" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>203</v>
@@ -6266,35 +6254,36 @@
     </row>
     <row r="116" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B117" s="4" t="s">
+      <c r="K116" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B117" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="K117" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="118" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B118" s="23" t="s">
+      <c r="D117" s="22"/>
+    </row>
+    <row r="118" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="13" t="s">
+        <v>882</v>
+      </c>
+      <c r="B118" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="D118" s="22"/>
+      <c r="D118" s="13"/>
     </row>
     <row r="119" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="13" t="s">
-        <v>882</v>
+        <v>74</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>203</v>
@@ -6303,7 +6292,7 @@
     </row>
     <row r="120" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="13" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>203</v>
@@ -6312,24 +6301,15 @@
     </row>
     <row r="121" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>203</v>
       </c>
       <c r="D121" s="13"/>
     </row>
-    <row r="122" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B122" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="D122" s="13"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:L68" xr:uid="{05A83487-31A5-894A-B1C5-9D57C8ECFC86}"/>
+  <autoFilter ref="A1:L67" xr:uid="{05A83487-31A5-894A-B1C5-9D57C8ECFC86}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -6623,7 +6603,7 @@
         <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C2" t="s">
         <v>87</v>
@@ -6652,7 +6632,7 @@
         <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C3" t="s">
         <v>87</v>
@@ -6681,7 +6661,7 @@
         <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C4" t="s">
         <v>92</v>
@@ -6710,7 +6690,7 @@
         <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C5" t="s">
         <v>92</v>
@@ -6739,7 +6719,7 @@
         <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C6" t="s">
         <v>86</v>
@@ -8027,22 +8007,22 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
     </row>
   </sheetData>
@@ -10328,7 +10308,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="39.83203125" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
   </cols>
@@ -10346,10 +10326,10 @@
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="45" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B2" t="s">
         <v>1049</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1050</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -10357,47 +10337,47 @@
         <v>1032</v>
       </c>
       <c r="B3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B4" s="48" t="s">
         <v>1069</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>1070</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B5" t="s">
         <v>1072</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1073</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="48" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B6" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B7" t="s">
         <v>1090</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1091</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B8" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -10405,12 +10385,12 @@
         <v>852</v>
       </c>
       <c r="B9" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B10" t="s">
         <v>854</v>
@@ -10418,7 +10398,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B11" t="s">
         <v>853</v>
@@ -10429,7 +10409,7 @@
         <v>851</v>
       </c>
       <c r="B12" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -10437,12 +10417,12 @@
         <v>490</v>
       </c>
       <c r="B13" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B14" t="s">
         <v>869</v>
@@ -10450,18 +10430,18 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="B15" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="B16" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
     </row>
   </sheetData>
@@ -10592,7 +10572,7 @@
         <v>66</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="E1" s="40" t="s">
         <v>67</v>
@@ -10658,7 +10638,7 @@
         <v>861</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="G4" s="31" t="s">
         <v>862</v>
@@ -10666,32 +10646,32 @@
     </row>
     <row r="5" spans="1:9" s="31" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="C5" s="31" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D5" s="31" t="s">
         <v>1150</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>1152</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="153" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B6" s="31" t="s">
         <v>1144</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>1146</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B7" s="31" t="s">
         <v>1145</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>1147</v>
-      </c>
       <c r="C7" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>851</v>
@@ -10706,7 +10686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F669E815-91F3-614D-A79B-23630F6A2A2E}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -10728,7 +10708,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="40" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="B1" s="40" t="s">
         <v>63</v>
@@ -10760,7 +10740,7 @@
     </row>
     <row r="2" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>84</v>
@@ -10786,7 +10766,7 @@
     </row>
     <row r="3" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B3" s="31" t="s">
         <v>85</v>
@@ -10835,13 +10815,13 @@
     </row>
     <row r="5" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B5" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="C5" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="G5" s="31" t="s">
         <v>99</v>
@@ -10849,13 +10829,13 @@
     </row>
     <row r="6" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B6" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="C6" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="G6" s="31" t="s">
         <v>99</v>
@@ -10863,13 +10843,13 @@
     </row>
     <row r="7" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B7" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="C7" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="G7" s="31" t="s">
         <v>99</v>
@@ -10883,13 +10863,13 @@
         <v>1012</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="G8" s="31" t="s">
         <v>99</v>
       </c>
       <c r="J8" s="31" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.2">
@@ -10897,16 +10877,16 @@
         <v>1032</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="C9" s="46" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="G9" s="31" t="s">
         <v>99</v>
       </c>
       <c r="J9" s="32" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.2">
@@ -10914,16 +10894,16 @@
         <v>1032</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="G10" s="31" t="s">
         <v>99</v>
       </c>
       <c r="J10" s="32" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.2">
@@ -10931,27 +10911,27 @@
         <v>1032</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="C11" s="46" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="G11" s="31" t="s">
         <v>99</v>
       </c>
       <c r="J11" s="32" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B12" s="49" t="s">
         <v>146</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="G12" s="31" t="s">
         <v>99</v>
@@ -10959,13 +10939,13 @@
     </row>
     <row r="13" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="G13" s="31" t="s">
         <v>99</v>
@@ -10973,13 +10953,13 @@
     </row>
     <row r="14" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="B14" s="48" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="G14" s="31" t="s">
         <v>99</v>
@@ -10987,13 +10967,13 @@
     </row>
     <row r="15" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B15" s="31" t="s">
         <v>1093</v>
       </c>
-      <c r="B15" s="31" t="s">
-        <v>1094</v>
-      </c>
       <c r="C15" s="31" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="G15" s="31" t="s">
         <v>99</v>
@@ -11001,13 +10981,13 @@
     </row>
     <row r="16" spans="1:10" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="G16" s="31" t="s">
         <v>99</v>
@@ -11080,7 +11060,7 @@
         <v>83</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -11088,7 +11068,7 @@
         <v>83</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -11827,7 +11807,7 @@
         <v>1012</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -11835,31 +11815,31 @@
         <v>1012</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" s="30" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B40" s="47" t="s">
         <v>1065</v>
-      </c>
-      <c r="B40" s="47" t="s">
-        <v>1066</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="30" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="30" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -11867,67 +11847,67 @@
         <v>146</v>
       </c>
       <c r="B43" s="30" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E43" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="30" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B44" s="48" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="E44" s="48" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="30" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B45" s="48" t="s">
         <v>1078</v>
       </c>
-      <c r="B45" s="48" t="s">
-        <v>1079</v>
-      </c>
       <c r="E45" s="48" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="30" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B46" s="48" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="E46" s="49" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="30" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B47" s="48" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="30" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B48" s="48" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="30" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B49" s="48" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
   </sheetData>
@@ -11971,7 +11951,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>51</v>
@@ -12018,7 +11998,7 @@
         <v>83</v>
       </c>
       <c r="B2" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C2" t="s">
         <v>487</v>
@@ -12052,7 +12032,7 @@
         <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C4" t="s">
         <v>86</v>
@@ -12066,7 +12046,7 @@
         <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C5" t="s">
         <v>87</v>
@@ -12080,7 +12060,7 @@
         <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C6" t="s">
         <v>92</v>
@@ -12094,19 +12074,19 @@
         <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C7" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="D7" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="G7" t="s">
         <v>262</v>
       </c>
       <c r="H7" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -12114,19 +12094,19 @@
         <v>83</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="K8" s="59"/>
       <c r="L8" s="59"/>
@@ -12137,19 +12117,19 @@
         <v>83</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="C9" s="58" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="K9" s="59"/>
       <c r="L9" s="59"/>
@@ -15450,7 +15430,7 @@
         <v>128</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -17859,16 +17839,16 @@
         <v>83</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="C4" s="30" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D4" s="30" t="s">
         <v>1129</v>
       </c>
-      <c r="D4" s="30" t="s">
-        <v>1131</v>
-      </c>
       <c r="E4" s="30" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -17876,16 +17856,16 @@
         <v>83</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -17893,16 +17873,16 @@
         <v>83</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>